<commit_message>
atualizacao do controle de vigencia
</commit_message>
<xml_diff>
--- a/database/tabela_uasg.xlsx
+++ b/database/tabela_uasg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63fbdbda17b5124d/Área de Trabalho/PyQt6/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63fbdbda17b5124d/Área de Trabalho/Programa git/pyqt6/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{37CE11E3-1A16-45F3-A72D-417DA1CA9224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E94752F-C39B-4522-B652-DD082B89C279}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{37CE11E3-1A16-45F3-A72D-417DA1CA9224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E1C3D92-7D1D-4CB5-8A53-2808B31F5CAB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,10 +227,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -268,7 +272,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -374,7 +378,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -516,7 +520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -527,7 +531,7 @@
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
comit gerar atas novo
</commit_message>
<xml_diff>
--- a/database/tabela_uasg.xlsx
+++ b/database/tabela_uasg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63fbdbda17b5124d/Área de Trabalho/Programa git/pyqt6/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Área de Trabalho\Programa PYQT6\pyqt6\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{37CE11E3-1A16-45F3-A72D-417DA1CA9224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E1C3D92-7D1D-4CB5-8A53-2808B31F5CAB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355006BA-B372-416F-96B2-0E92CE61CE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="OBJ_PREFIX_DWT821_com_zimbra_date">#REF!</definedName>
     <definedName name="OBJ_PREFIX_DWT822_com_zimbra_date">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>uasg</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>CENTRO DE INTENDÊNCIA DA MARINHA EM BRASÍLIA</t>
+  </si>
+  <si>
+    <t>TESTE</t>
   </si>
 </sst>
 </file>
@@ -225,10 +228,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,21 +527,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ10"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A12" sqref="A12:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="81.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="2" customWidth="1"/>
-    <col min="4" max="1024" width="11.6640625" style="1"/>
+    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="81.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" style="2" customWidth="1"/>
+    <col min="4" max="1024" width="11.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -553,7 +552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>787000</v>
       </c>
@@ -564,7 +563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>787010</v>
       </c>
@@ -575,7 +574,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>787310</v>
       </c>
@@ -586,7 +585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>787320</v>
       </c>
@@ -597,7 +596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>787200</v>
       </c>
@@ -608,7 +607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>787900</v>
       </c>
@@ -619,7 +618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>787400</v>
       </c>
@@ -630,7 +629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>787330</v>
       </c>
@@ -641,7 +640,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>787700</v>
       </c>
@@ -649,6 +648,17 @@
         <v>15</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>787701</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
inserir tabela na ata
</commit_message>
<xml_diff>
--- a/database/tabela_uasg.xlsx
+++ b/database/tabela_uasg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Documents\Nova pasta\projeto_licitacao360\licitacao360\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive\Área de Trabalho\projeto_licitacao360\licitacao360\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A14027-544C-438C-B257-7928818D1F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7718EA-B64A-47D1-A7E9-24CE0F7BA02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -88,24 +88,12 @@
     <t>CENTRO DE INTENDÊNCIA DA MARINHA EM BRASÍLIA</t>
   </si>
   <si>
-    <t>om_extenso</t>
-  </si>
-  <si>
-    <t>om</t>
-  </si>
-  <si>
     <t>SETDIS</t>
   </si>
   <si>
-    <t>CIBRA</t>
-  </si>
-  <si>
     <t>CFATOC</t>
   </si>
   <si>
-    <t>CFBRA</t>
-  </si>
-  <si>
     <t>GRFBRA</t>
   </si>
   <si>
@@ -115,13 +103,25 @@
     <t>ERMBRA</t>
   </si>
   <si>
-    <t>CFGOO</t>
-  </si>
-  <si>
     <t>HOSBRA</t>
   </si>
   <si>
     <t>indicativo_om</t>
+  </si>
+  <si>
+    <t>orgao_responsavel</t>
+  </si>
+  <si>
+    <t>sigla_om</t>
+  </si>
+  <si>
+    <t>CITBRA</t>
+  </si>
+  <si>
+    <t>CFGOIA</t>
+  </si>
+  <si>
+    <t>CPFBRA</t>
   </si>
 </sst>
 </file>
@@ -150,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -173,50 +173,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -225,20 +186,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,156 +510,156 @@
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R23" sqref="R22:R23"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="53.08984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.36328125" style="1" customWidth="1"/>
-    <col min="5" max="1024" width="11.6328125" style="1"/>
+    <col min="1" max="1" width="17.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="53.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="1" customWidth="1"/>
+    <col min="5" max="1024" width="11.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="3">
         <v>787000</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>787010</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>787310</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>787320</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>787200</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>787900</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>787400</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>787330</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>787700</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
+      <c r="D10" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>